<commit_message>
[template] 新增 & 修改(40021 / 40022)
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40021.xlsx
+++ b/PhoenixCI/Excel_Template/40021.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\需求單\1071230\ExcelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJSOFT\source\repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961470DD-1719-4F2F-AB01-81A344C436F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="-30" windowWidth="7650" windowHeight="7335" tabRatio="962" activeTab="2"/>
+    <workbookView xWindow="3045" yWindow="-30" windowWidth="7650" windowHeight="7335" tabRatio="962" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Span參數日狀況表(一)" sheetId="26" r:id="rId1"/>
@@ -27,7 +28,14 @@
     <definedName name="XX_TEJ5">#REF!</definedName>
     <definedName name="XX_TEJ6">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -227,10 +235,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>變動幅度已達 10% 之得調整標準，建議事項如「SPAN參數調整審核會議記錄」.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>經　辦：______________          覆核：______________             經理：______________</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -399,60 +403,6 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>之得調整標準，建議事項如「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>SPAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>參數調整審核會議記錄」</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
       <t>除作業事項</t>
     </r>
     <r>
@@ -714,18 +664,142 @@
     <t>ETC</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="4"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">10% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>之得調整標準，建議事項如「</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SPAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>參數調整審核會議紀錄」</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>變動幅度已達</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="4"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">10% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>之得調整標準，建議事項如「</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>SPAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>參數調整審核會議紀錄」</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="0.0%"/>
     <numFmt numFmtId="179" formatCode="0.0%_);\(0.0%\);*-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -855,6 +929,17 @@
       <family val="4"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="4"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -909,7 +994,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1095,12 +1180,21 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1115,14 +1209,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
-    <cellStyle name="一般 3" xfId="2"/>
-    <cellStyle name="百分比 2" xfId="3"/>
-    <cellStyle name="百分比 3" xfId="4"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="百分比 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="百分比 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1226,6 +1323,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1261,6 +1375,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1436,12 +1567,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1457,12 +1588,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="53" t="s">
@@ -1584,7 +1715,7 @@
     </row>
     <row r="14" spans="1:6" ht="25.5" customHeight="1">
       <c r="B14" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="37" t="e">
         <f>#REF!</f>
@@ -1600,7 +1731,7 @@
     </row>
     <row r="15" spans="1:6" ht="25.5" customHeight="1">
       <c r="B15" s="64" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" s="37" t="e">
         <f>#REF!</f>
@@ -1677,8 +1808,8 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
-        <v>27</v>
+      <c r="B23" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
@@ -1704,7 +1835,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -1750,12 +1881,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1769,19 +1900,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="46.5" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="2" spans="1:9" ht="16.5">
       <c r="B2" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.95" customHeight="1">
@@ -1807,7 +1939,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1941,10 +2073,10 @@
     <row r="11" spans="1:9" ht="16.5">
       <c r="A11" s="22"/>
       <c r="B11" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -1956,7 +2088,7 @@
     <row r="12" spans="1:9">
       <c r="A12" s="22"/>
       <c r="B12" s="58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="59">
         <v>0.88</v>
@@ -2059,7 +2191,7 @@
     <row r="21" spans="1:9" ht="16.5">
       <c r="A21" s="22"/>
       <c r="B21" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -2093,7 +2225,7 @@
         <v>7</v>
       </c>
       <c r="I22" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2248,10 +2380,10 @@
     <row r="30" spans="1:9" ht="16.5">
       <c r="A30" s="22"/>
       <c r="B30" s="61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -2263,7 +2395,7 @@
     <row r="31" spans="1:9">
       <c r="A31" s="22"/>
       <c r="B31" s="62" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="63" t="e">
         <f>#REF!</f>
@@ -2367,7 +2499,7 @@
     <row r="40" spans="1:9" ht="16.5">
       <c r="A40" s="22"/>
       <c r="B40" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
@@ -2380,7 +2512,7 @@
     <row r="41" spans="1:9" ht="16.5">
       <c r="A41" s="22"/>
       <c r="B41" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
@@ -2414,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="I42" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2549,16 +2681,16 @@
     <row r="50" spans="1:16" ht="15.95" customHeight="1">
       <c r="A50" s="32"/>
       <c r="B50" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="15.95" customHeight="1">
       <c r="A51" s="32"/>
       <c r="B51" s="58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C51" s="60" t="e">
         <f>ROUNDUP((C31-C12)/C12,3)</f>
@@ -2577,10 +2709,10 @@
     </row>
     <row r="53" spans="1:16" ht="16.5">
       <c r="A53" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>36</v>
       </c>
       <c r="C53" s="30"/>
       <c r="D53" s="30"/>
@@ -2598,7 +2730,7 @@
     <row r="55" spans="1:16" ht="16.5">
       <c r="A55" s="22"/>
       <c r="B55" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -2613,21 +2745,21 @@
     </row>
     <row r="56" spans="1:16" ht="31.5" customHeight="1">
       <c r="A56" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B56" s="69"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
+        <v>37</v>
+      </c>
+      <c r="B56" s="72"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="72"/>
+      <c r="F56" s="72"/>
+      <c r="G56" s="72"/>
+      <c r="H56" s="72"/>
       <c r="I56" s="46"/>
     </row>
     <row r="57" spans="1:16" ht="16.5">
       <c r="A57" s="22"/>
-      <c r="B57" s="29" t="s">
-        <v>39</v>
+      <c r="B57" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="33"/>
@@ -2645,26 +2777,26 @@
       <c r="A59" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="C59" s="68"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="68"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
+      <c r="B59" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
+      <c r="G59" s="71"/>
+      <c r="H59" s="71"/>
       <c r="I59" s="45"/>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="32"/>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
       <c r="I60" s="45"/>
     </row>
     <row r="61" spans="1:16">
@@ -2672,7 +2804,7 @@
     </row>
     <row r="62" spans="1:16" ht="16.5">
       <c r="A62" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" ht="15.95" customHeight="1"/>
@@ -2699,14 +2831,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J1"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2725,20 +2857,20 @@
   <sheetData>
     <row r="1" spans="1:10" ht="43.5" customHeight="1">
       <c r="A1" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
     </row>
     <row r="2" spans="1:10" ht="16.5">
       <c r="B2" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.95" customHeight="1">
@@ -2764,7 +2896,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2898,10 +3030,10 @@
     <row r="11" spans="1:10" ht="16.5">
       <c r="A11" s="22"/>
       <c r="B11" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -2913,7 +3045,7 @@
     <row r="12" spans="1:10">
       <c r="A12" s="22"/>
       <c r="B12" s="58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="59">
         <v>0.5</v>
@@ -3038,7 +3170,7 @@
     <row r="23" spans="1:9" ht="16.5">
       <c r="A23" s="22"/>
       <c r="B23" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
@@ -3072,7 +3204,7 @@
         <v>7</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3227,10 +3359,10 @@
     <row r="32" spans="1:9" ht="16.5">
       <c r="A32" s="22"/>
       <c r="B32" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -3242,7 +3374,7 @@
     <row r="33" spans="1:9">
       <c r="A33" s="22"/>
       <c r="B33" s="58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="59" t="e">
         <f>#REF!</f>
@@ -3346,7 +3478,7 @@
     <row r="42" spans="1:9" ht="16.5">
       <c r="A42" s="22"/>
       <c r="B42" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -3393,7 +3525,7 @@
         <v>7</v>
       </c>
       <c r="I44" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3535,10 +3667,10 @@
     <row r="52" spans="1:16" ht="16.5">
       <c r="A52" s="28"/>
       <c r="B52" s="57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="25"/>
@@ -3549,7 +3681,7 @@
     <row r="53" spans="1:16">
       <c r="A53" s="28"/>
       <c r="B53" s="58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C53" s="60" t="e">
         <f>ROUNDUP((C33-C12)/C12,3)</f>
@@ -3573,10 +3705,10 @@
     </row>
     <row r="55" spans="1:16" ht="16.5">
       <c r="A55" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="29" t="s">
         <v>35</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>36</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -3588,7 +3720,7 @@
       <c r="B56" s="29"/>
       <c r="C56" s="30"/>
       <c r="D56" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="31"/>
@@ -3596,7 +3728,7 @@
     <row r="57" spans="1:16" ht="16.5">
       <c r="A57" s="22"/>
       <c r="B57" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
@@ -3611,7 +3743,7 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="48"/>
       <c r="C58" s="29"/>
@@ -3623,8 +3755,8 @@
     </row>
     <row r="59" spans="1:16" ht="16.5">
       <c r="A59" s="22"/>
-      <c r="B59" s="29" t="s">
-        <v>39</v>
+      <c r="B59" s="66" t="s">
+        <v>50</v>
       </c>
       <c r="C59" s="22"/>
       <c r="D59" s="33"/>
@@ -3642,27 +3774,27 @@
       <c r="A61" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="C61" s="71"/>
-      <c r="D61" s="71"/>
-      <c r="E61" s="71"/>
-      <c r="F61" s="71"/>
-      <c r="G61" s="71"/>
-      <c r="H61" s="71"/>
-      <c r="I61" s="71"/>
+      <c r="B61" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="74"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="74"/>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="32"/>
-      <c r="B62" s="71"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="71"/>
-      <c r="F62" s="71"/>
-      <c r="G62" s="71"/>
-      <c r="H62" s="71"/>
-      <c r="I62" s="71"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="74"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="74"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="32"/>
@@ -3682,7 +3814,7 @@
     </row>
     <row r="67" spans="1:5" ht="16.5">
       <c r="A67" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.95" customHeight="1"/>

</xml_diff>

<commit_message>
[template] 40021(修改) [Modify] 40210
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40021.xlsx
+++ b/PhoenixCI/Excel_Template/40021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJSOFT\source\repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961470DD-1719-4F2F-AB01-81A344C436F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB13C08-DE76-46A5-86CA-3D19FA159414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3045" yWindow="-30" windowWidth="7650" windowHeight="7335" tabRatio="962" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -665,128 +665,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="4"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">10% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>之得調整標準，建議事項如「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>SPAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>參數調整審核會議紀錄」</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
+    <t>變動幅度已達 10% 之得調整標準，建議事項如「SPAN參數調整審核會議紀錄」.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>變動幅度已達 10% 之得調整標準，建議事項如「SPAN參數調整審核會議紀錄」.</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>變動幅度已達</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="4"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">10% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>之得調整標準，建議事項如「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>SPAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>參數調整審核會議紀錄」</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -799,7 +683,7 @@
     <numFmt numFmtId="178" formatCode="0.0%"/>
     <numFmt numFmtId="179" formatCode="0.0%_);\(0.0%\);*-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -929,17 +813,6 @@
       <family val="4"/>
       <charset val="136"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="4"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="4"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -994,7 +867,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1180,11 +1053,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1203,9 +1073,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1572,7 +1439,7 @@
   <dimension ref="A2:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1588,12 +1455,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="E3" s="67"/>
-      <c r="F3" s="68"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="53" t="s">
@@ -1809,7 +1676,7 @@
     <row r="23" spans="1:7">
       <c r="A23" s="5"/>
       <c r="B23" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
@@ -1886,7 +1753,7 @@
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+      <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1894,7 +1761,7 @@
     <col min="1" max="1" width="5.125" style="13" customWidth="1"/>
     <col min="2" max="2" width="18.125" style="13" customWidth="1"/>
     <col min="3" max="8" width="11.625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="6.75" style="13" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.75" style="13" hidden="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
@@ -1906,10 +1773,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="53"/>
-      <c r="F1" s="65"/>
+      <c r="F1" s="73"/>
       <c r="G1" s="73"/>
       <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" ht="16.5">
       <c r="B2" s="15" t="s">
@@ -2747,19 +2614,19 @@
       <c r="A56" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="72"/>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
+      <c r="F56" s="71"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
       <c r="I56" s="46"/>
     </row>
     <row r="57" spans="1:16" ht="16.5">
       <c r="A57" s="22"/>
-      <c r="B57" s="66" t="s">
-        <v>50</v>
+      <c r="B57" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C57" s="22"/>
       <c r="D57" s="33"/>
@@ -2777,26 +2644,26 @@
       <c r="A59" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="70" t="s">
+      <c r="B59" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C59" s="71"/>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
-      <c r="F59" s="71"/>
-      <c r="G59" s="71"/>
-      <c r="H59" s="71"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="70"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
       <c r="I59" s="45"/>
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="32"/>
-      <c r="B60" s="71"/>
-      <c r="C60" s="71"/>
-      <c r="D60" s="71"/>
-      <c r="E60" s="71"/>
-      <c r="F60" s="71"/>
-      <c r="G60" s="71"/>
-      <c r="H60" s="71"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
       <c r="I60" s="45"/>
     </row>
     <row r="61" spans="1:16">
@@ -2814,7 +2681,7 @@
   <mergeCells count="3">
     <mergeCell ref="B59:H60"/>
     <mergeCell ref="B56:H56"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.19685039370078741" right="0.23622047244094491" top="1.0236220472440944" bottom="0.23622047244094491" header="0.27559055118110237" footer="0.23622047244094491"/>
@@ -2837,8 +2704,8 @@
   </sheetPr>
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2864,9 +2731,9 @@
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
     </row>
     <row r="2" spans="1:10" ht="16.5">
       <c r="B2" s="15" t="s">
@@ -3755,8 +3622,8 @@
     </row>
     <row r="59" spans="1:16" ht="16.5">
       <c r="A59" s="22"/>
-      <c r="B59" s="66" t="s">
-        <v>50</v>
+      <c r="B59" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C59" s="22"/>
       <c r="D59" s="33"/>
@@ -3774,27 +3641,27 @@
       <c r="A61" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B61" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="C61" s="74"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
-      <c r="F61" s="74"/>
-      <c r="G61" s="74"/>
-      <c r="H61" s="74"/>
-      <c r="I61" s="74"/>
+      <c r="C61" s="72"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="72"/>
+      <c r="F61" s="72"/>
+      <c r="G61" s="72"/>
+      <c r="H61" s="72"/>
+      <c r="I61" s="72"/>
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="32"/>
-      <c r="B62" s="74"/>
-      <c r="C62" s="74"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="74"/>
+      <c r="B62" s="72"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="72"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="72"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
+      <c r="I62" s="72"/>
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="32"/>

</xml_diff>